<commit_message>
Some more separating logic from view
</commit_message>
<xml_diff>
--- a/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
+++ b/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <r>
       <rPr>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t xml:space="preserve">Trying to implement a better dependency injection for all types. Finding it hard to make it work. Somehow I always get stuck trying things like an abstractFactory and using protocols to inject dependencies. So far I’ve only been able to inject dependencies by properties and initialisers through a RootViewController, but I’m sure there is a better way. I’ve tried to separate more code from the view controller classes, into a view model to conform to MVVM Pattern. Added constants. Removed force unwrapping or used Guard != nil for safer code. Added more protocols to Service layer. </t>
+  </si>
+  <si>
+    <t>Minor adjustments separation</t>
+  </si>
+  <si>
+    <t>Created a DetailViewModel to separate logic even more from view.</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -2131,10 +2137,18 @@
       <c r="F18" s="16"/>
     </row>
     <row r="19" ht="17" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
+      <c r="A19" t="s" s="11">
+        <v>37</v>
+      </c>
+      <c r="B19" s="12">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13">
+        <v>44621</v>
+      </c>
+      <c r="D19" t="s" s="14">
+        <v>38</v>
+      </c>
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
     </row>
@@ -2220,11 +2234,11 @@
     </row>
     <row r="30" ht="16.25" customHeight="1">
       <c r="A30" t="s" s="26">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B30" s="27">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="29"/>

</xml_diff>

<commit_message>
Replaced segue method to new instantiateViewController method for cleaner code
</commit_message>
<xml_diff>
--- a/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
+++ b/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Created a DetailViewModel to separate logic even more from view.</t>
+  </si>
+  <si>
+    <t>Replaced segue to detail view</t>
+  </si>
+  <si>
+    <t>Replaced segue to detailview with new method storyboard.instantiateViewController. Removed optional HouseManager (view model). Made code a bit cleaner.</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -2153,10 +2159,18 @@
       <c r="F19" s="16"/>
     </row>
     <row r="20" ht="17" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
+      <c r="A20" t="s" s="11">
+        <v>39</v>
+      </c>
+      <c r="B20" s="12">
+        <v>1</v>
+      </c>
+      <c r="C20" s="13">
+        <v>44621</v>
+      </c>
+      <c r="D20" t="s" s="14">
+        <v>40</v>
+      </c>
       <c r="E20" s="15"/>
       <c r="F20" s="16"/>
     </row>
@@ -2234,11 +2248,11 @@
     </row>
     <row r="30" ht="16.25" customHeight="1">
       <c r="A30" t="s" s="26">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B30" s="27">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="29"/>

</xml_diff>

<commit_message>
Made proper MVVM pattern for both HousesViewController and DetailViewController
</commit_message>
<xml_diff>
--- a/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
+++ b/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <r>
       <rPr>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Replaced segue to detailview with new method storyboard.instantiateViewController. Removed optional HouseManager (view model). Made code a bit cleaner.</t>
+  </si>
+  <si>
+    <t>Just some more refactoring</t>
+  </si>
+  <si>
+    <t>Added an infoViewModel for consistency. Took out the houses property in HousesViewController and made use of the HouseManager.houses. Same for chosenHouse in DetailViewController. Now I think it’s proper use of the MVVM pattern.</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -2158,7 +2164,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" ht="17" customHeight="1">
+    <row r="20" ht="28.45" customHeight="1">
       <c r="A20" t="s" s="11">
         <v>39</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="13">
-        <v>44621</v>
+        <v>44622</v>
       </c>
       <c r="D20" t="s" s="14">
         <v>40</v>
@@ -2174,11 +2180,19 @@
       <c r="E20" s="15"/>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" ht="17" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
+    <row r="21" ht="43" customHeight="1">
+      <c r="A21" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="B21" s="12">
+        <v>1</v>
+      </c>
+      <c r="C21" s="13">
+        <v>44622</v>
+      </c>
+      <c r="D21" t="s" s="14">
+        <v>42</v>
+      </c>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
     </row>
@@ -2248,11 +2262,11 @@
     </row>
     <row r="30" ht="16.25" customHeight="1">
       <c r="A30" t="s" s="26">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="27">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="29"/>

</xml_diff>

<commit_message>
Fixed bug in searching system. Removed coredata singleton
</commit_message>
<xml_diff>
--- a/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
+++ b/RealEstateDTT/Log/DTT-Test-Hour-Log-1_updated_bonus Patrick Rugebregt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <r>
       <rPr>
@@ -167,6 +167,12 @@
     <t>Added an infoViewModel for consistency. Took out the houses property in HousesViewController and made use of the HouseManager.houses. Same for chosenHouse in DetailViewController. Now I think it’s proper use of the MVVM pattern.</t>
   </si>
   <si>
+    <t>Fixed bug and removed singleton core data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Had a small bug in the sent version where there were 2 instances of coredatamanager. First fixed it by making it a singleton, now I used the AppDelegate to reference the core data instance. Fixed search bug (original filter list of houses was being updated to contain only filtered results) </t>
+  </si>
+  <si>
     <t>Total amount of hours</t>
   </si>
 </sst>
@@ -174,9 +180,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="60" formatCode="0.0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -573,7 +580,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -624,6 +631,9 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="60" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
@@ -2196,11 +2206,19 @@
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" ht="17" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
+    <row r="22" ht="43" customHeight="1">
+      <c r="A22" t="s" s="11">
+        <v>43</v>
+      </c>
+      <c r="B22" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="13">
+        <v>44623</v>
+      </c>
+      <c r="D22" t="s" s="14">
+        <v>44</v>
+      </c>
       <c r="E22" s="15"/>
       <c r="F22" s="16"/>
     </row>
@@ -2245,57 +2263,57 @@
       <c r="F27" s="16"/>
     </row>
     <row r="28" ht="17" customHeight="1">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="15"/>
       <c r="F28" s="16"/>
     </row>
     <row r="29" ht="16.25" customHeight="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="25"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="26"/>
     </row>
     <row r="30" ht="16.25" customHeight="1">
-      <c r="A30" t="s" s="26">
-        <v>43</v>
-      </c>
-      <c r="B30" s="27">
+      <c r="A30" t="s" s="27">
+        <v>45</v>
+      </c>
+      <c r="B30" s="28">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>14.5</v>
-      </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="25"/>
+        <v>15</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="26"/>
     </row>
     <row r="31" ht="16.25" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="25"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" ht="16.25" customHeight="1">
-      <c r="A32" s="33"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="25"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" ht="16.25" customHeight="1">
-      <c r="A33" s="34"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>